<commit_message>
Lab Notebook update - fixed LN repository
</commit_message>
<xml_diff>
--- a/Data/LN_Repository.xlsx
+++ b/Data/LN_Repository.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofcambridgecloud-my.sharepoint.com/personal/cm2162_cam_ac_uk/Documents/Lab Notebook/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="8_{A0DFC8DC-65E8-5244-94FE-8C36CB89D114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB33018C-9EFD-6848-833D-794B58F6795D}"/>
+  <xr:revisionPtr revIDLastSave="227" documentId="8_{A0DFC8DC-65E8-5244-94FE-8C36CB89D114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9EE5C59E-3CF2-7747-A06D-53ABE07A11CC}"/>
   <bookViews>
-    <workbookView xWindow="34940" yWindow="-1360" windowWidth="27640" windowHeight="16400" xr2:uid="{C3A89E94-CACF-C147-841F-3BBFCDBF8367}"/>
+    <workbookView xWindow="32640" yWindow="-1220" windowWidth="29400" windowHeight="17200" xr2:uid="{C3A89E94-CACF-C147-841F-3BBFCDBF8367}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="55">
   <si>
     <t>Location</t>
   </si>
@@ -69,16 +70,154 @@
   </si>
   <si>
     <t>710 NM - A20 Mouse Experiment</t>
+  </si>
+  <si>
+    <t>RBL1</t>
+  </si>
+  <si>
+    <t>RBL1 PDX</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - </t>
+  </si>
+  <si>
+    <t>Ramos BC 5</t>
+  </si>
+  <si>
+    <t>Ramos BC Pool 5</t>
+  </si>
+  <si>
+    <t>Ramos BC 1</t>
+  </si>
+  <si>
+    <t>Ramos Barcode Pool 1</t>
+  </si>
+  <si>
+    <t>A20 Cell Pool</t>
+  </si>
+  <si>
+    <t>N2 BC</t>
+  </si>
+  <si>
+    <t>N2 Barcoded pool</t>
+  </si>
+  <si>
+    <t>B-IP-723 NM</t>
+  </si>
+  <si>
+    <t>B-IP-724-1L</t>
+  </si>
+  <si>
+    <t>B-IP-723-2L</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -</t>
+  </si>
+  <si>
+    <t>Ramos BC 3</t>
+  </si>
+  <si>
+    <t>Ramos Barcode Pool 3</t>
+  </si>
+  <si>
+    <t>N4</t>
+  </si>
+  <si>
+    <t>N4 PDX pool</t>
+  </si>
+  <si>
+    <t>BLLW</t>
+  </si>
+  <si>
+    <t>BLLW PDX Pool</t>
+  </si>
+  <si>
+    <t>N2 BC 5</t>
+  </si>
+  <si>
+    <t>N2 barcode pool 5</t>
+  </si>
+  <si>
+    <t>Ramos Barcode Pool 5</t>
+  </si>
+  <si>
+    <t>723-2R</t>
+  </si>
+  <si>
+    <t>723-1L</t>
+  </si>
+  <si>
+    <t>Ramos BC 6</t>
+  </si>
+  <si>
+    <t>Ramos Barcode Pool 6</t>
+  </si>
+  <si>
+    <t>04/16/2024</t>
+  </si>
+  <si>
+    <t>Ramos Barcode Pool 1 *</t>
+  </si>
+  <si>
+    <t>Ramos RTX CDC Baseline</t>
+  </si>
+  <si>
+    <t>C4 DP2</t>
+  </si>
+  <si>
+    <t>C5 DP2</t>
+  </si>
+  <si>
+    <t>R3 DP2</t>
+  </si>
+  <si>
+    <t>C6 DP2</t>
+  </si>
+  <si>
+    <t>C1 DP2</t>
+  </si>
+  <si>
+    <t>C2 DP2</t>
+  </si>
+  <si>
+    <t>Ramos RTX CDC C1-DP2</t>
+  </si>
+  <si>
+    <t>Ramos RTX CDC C2-DP2</t>
+  </si>
+  <si>
+    <t>Ramos RTX CDC C4-DP2</t>
+  </si>
+  <si>
+    <t>Ramos RTX CDC C5-DP2</t>
+  </si>
+  <si>
+    <t>Ramos RTX CDC R3-DP2</t>
+  </si>
+  <si>
+    <t>Ramos RTX CDC C6-DP2</t>
+  </si>
+  <si>
+    <t>Ramos RTX CDC C3-DP2</t>
+  </si>
+  <si>
+    <t>C3 DP2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -104,9 +243,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -122,6 +262,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -441,19 +585,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D715BC7-5079-8340-B8F7-7A3D7EFA53DC}">
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E104" sqref="E104"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -463,11 +607,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -477,151 +621,157 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="D3" t="str">
+        <f>TEXT(Sheet2!A3, "dd/mm/yyyy")</f>
+        <v>12/06/2024</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="D4" t="str">
+        <f>TEXT(Sheet2!A4, "dd/mm/yyyy")</f>
+        <v>12/06/2024</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="D5" t="str">
+        <f>TEXT(Sheet2!A5, "dd/mm/yyyy")</f>
+        <v>12/06/2024</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -631,11 +781,11 @@
       <c r="C13" t="s">
         <v>6</v>
       </c>
-      <c r="D13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D13" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -645,11 +795,11 @@
       <c r="C14" t="s">
         <v>6</v>
       </c>
-      <c r="D14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D14" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -659,11 +809,11 @@
       <c r="C15" t="s">
         <v>6</v>
       </c>
-      <c r="D15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D15" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -673,11 +823,11 @@
       <c r="C16" t="s">
         <v>6</v>
       </c>
-      <c r="D16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D16" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -687,11 +837,11 @@
       <c r="C17" t="s">
         <v>6</v>
       </c>
-      <c r="D17" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D17" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -701,11 +851,12 @@
       <c r="C18" t="s">
         <v>6</v>
       </c>
-      <c r="D18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -715,11 +866,11 @@
       <c r="C19" t="s">
         <v>6</v>
       </c>
-      <c r="D19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D19" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -729,11 +880,12 @@
       <c r="C20" t="s">
         <v>6</v>
       </c>
-      <c r="D20" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -743,11 +895,11 @@
       <c r="C21" t="s">
         <v>6</v>
       </c>
-      <c r="D21" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D21" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -757,11 +909,12 @@
       <c r="C22" t="s">
         <v>6</v>
       </c>
-      <c r="D22" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -771,11 +924,12 @@
       <c r="C23" t="s">
         <v>6</v>
       </c>
-      <c r="D23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -785,11 +939,12 @@
       <c r="C24" t="s">
         <v>6</v>
       </c>
-      <c r="D24" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -799,11 +954,12 @@
       <c r="C25" t="s">
         <v>6</v>
       </c>
-      <c r="D25" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -813,11 +969,11 @@
       <c r="C26" t="s">
         <v>6</v>
       </c>
-      <c r="D26" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D26" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -827,11 +983,11 @@
       <c r="C27" t="s">
         <v>6</v>
       </c>
-      <c r="D27" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D27" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -841,11 +997,11 @@
       <c r="C28" t="s">
         <v>6</v>
       </c>
-      <c r="D28" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D28" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -855,11 +1011,12 @@
       <c r="C29" t="s">
         <v>6</v>
       </c>
-      <c r="D29" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -869,11 +1026,12 @@
       <c r="C30" t="s">
         <v>6</v>
       </c>
-      <c r="D30" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -883,137 +1041,158 @@
       <c r="C31" t="s">
         <v>6</v>
       </c>
-      <c r="D31" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C32" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="D32" t="str">
+        <f>TEXT(Sheet2!A32, "dd/mm/yyyy")</f>
+        <v>12/06/2024</v>
+      </c>
+      <c r="E32" s="1"/>
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C33" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="D33" t="str">
+        <f>TEXT(Sheet2!A33, "dd/mm/yyyy")</f>
+        <v>04/01/2023</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C34" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="D34" t="str">
+        <f>TEXT(Sheet2!A34, "dd/mm/yyyy")</f>
+        <v>16/07/2024</v>
+      </c>
+      <c r="E34" s="1"/>
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C35" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="D35" t="str">
+        <f>TEXT(Sheet2!A35, "dd/mm/yyyy")</f>
+        <v>12/06/2024</v>
+      </c>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C36" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="D36" t="str">
+        <f>TEXT(Sheet2!A36, "dd/mm/yyyy")</f>
+        <v>04/06/2024</v>
+      </c>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C37" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="D37" t="str">
+        <f>TEXT(Sheet2!A37, "dd/mm/yyyy")</f>
+        <v>12/06/2024</v>
+      </c>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="D38" t="str">
+        <f>TEXT(Sheet2!A38, "dd/mm/yyyy")</f>
+        <v>12/06/2024</v>
+      </c>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C39" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="D39" t="str">
+        <f>TEXT(Sheet2!A39, "dd/mm/yyyy")</f>
+        <v>04/16/2024</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="C40" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="D40" t="str">
+        <f>TEXT(Sheet2!A40, "dd/mm/yyyy")</f>
+        <v>04/16/2024</v>
+      </c>
+      <c r="H40" s="1"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1023,11 +1202,11 @@
       <c r="C41" t="s">
         <v>6</v>
       </c>
-      <c r="D41" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D41" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1037,11 +1216,11 @@
       <c r="C42" t="s">
         <v>6</v>
       </c>
-      <c r="D42" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D42" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1051,11 +1230,11 @@
       <c r="C43" t="s">
         <v>6</v>
       </c>
-      <c r="D43" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D43" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1065,11 +1244,11 @@
       <c r="C44" t="s">
         <v>6</v>
       </c>
-      <c r="D44" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D44" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1079,11 +1258,11 @@
       <c r="C45" t="s">
         <v>6</v>
       </c>
-      <c r="D45" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D45" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1093,11 +1272,11 @@
       <c r="C46" t="s">
         <v>6</v>
       </c>
-      <c r="D46" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D46" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1107,11 +1286,11 @@
       <c r="C47" t="s">
         <v>6</v>
       </c>
-      <c r="D47" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D47" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1121,7 +1300,7 @@
       <c r="C48" t="s">
         <v>6</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1135,7 +1314,7 @@
       <c r="C49" t="s">
         <v>6</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1149,7 +1328,7 @@
       <c r="C50" t="s">
         <v>6</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1163,7 +1342,7 @@
       <c r="C51" t="s">
         <v>6</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1172,13 +1351,14 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C52" t="s">
-        <v>6</v>
-      </c>
-      <c r="D52" t="s">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="D52" t="str">
+        <f>TEXT(Sheet2!A52, "dd/mm/yyyy")</f>
+        <v>31/07/2023</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -1186,13 +1366,14 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C53" t="s">
-        <v>6</v>
-      </c>
-      <c r="D53" t="s">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="D53" t="str">
+        <f>TEXT(Sheet2!A53, "dd/mm/yyyy")</f>
+        <v>31/07/2024</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -1200,13 +1381,14 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C54" t="s">
-        <v>6</v>
-      </c>
-      <c r="D54" t="s">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="D54" t="str">
+        <f>TEXT(Sheet2!A54, "dd/mm/yyyy")</f>
+        <v>31/07/2024</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -1214,13 +1396,14 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="C55" t="s">
-        <v>6</v>
-      </c>
-      <c r="D55" t="s">
-        <v>6</v>
+        <v>30</v>
+      </c>
+      <c r="D55" t="str">
+        <f>TEXT(Sheet2!A55, "dd/mm/yyyy")</f>
+        <v>31/07/2024</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -1228,13 +1411,14 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="C56" t="s">
-        <v>6</v>
-      </c>
-      <c r="D56" t="s">
-        <v>6</v>
+        <v>30</v>
+      </c>
+      <c r="D56" t="str">
+        <f>TEXT(Sheet2!A56, "dd/mm/yyyy")</f>
+        <v>31/07/2024</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -1242,13 +1426,14 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="C57" t="s">
-        <v>6</v>
-      </c>
-      <c r="D57" t="s">
-        <v>6</v>
+        <v>28</v>
+      </c>
+      <c r="D57" t="str">
+        <f>TEXT(Sheet2!A57, "dd/mm/yyyy")</f>
+        <v>07/11/2023</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -1256,13 +1441,14 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="C58" t="s">
-        <v>6</v>
-      </c>
-      <c r="D58" t="s">
-        <v>6</v>
+        <v>28</v>
+      </c>
+      <c r="D58" t="str">
+        <f>TEXT(Sheet2!A58, "dd/mm/yyyy")</f>
+        <v>07/11/2023</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -1270,13 +1456,14 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C59" t="s">
-        <v>6</v>
-      </c>
-      <c r="D59" t="s">
-        <v>6</v>
+        <v>20</v>
+      </c>
+      <c r="D59" t="str">
+        <f>TEXT(Sheet2!A59, "dd/mm/yyyy")</f>
+        <v>11/05/2023</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -1284,13 +1471,14 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="C60" t="s">
-        <v>6</v>
-      </c>
-      <c r="D60" t="s">
-        <v>6</v>
+        <v>32</v>
+      </c>
+      <c r="D60" t="str">
+        <f>TEXT(Sheet2!A60, "dd/mm/yyyy")</f>
+        <v>29/04/2024</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -1298,13 +1486,14 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C61" t="s">
-        <v>6</v>
-      </c>
-      <c r="D61" t="s">
-        <v>6</v>
+        <v>18</v>
+      </c>
+      <c r="D61" t="str">
+        <f>TEXT(Sheet2!A61, "dd/mm/yyyy")</f>
+        <v>13/10/2024</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -1312,13 +1501,14 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C62" t="s">
-        <v>6</v>
-      </c>
-      <c r="D62" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="D62" t="str">
+        <f>TEXT(Sheet2!A62, "dd/mm/yyyy")</f>
+        <v>13/10/2024</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -1331,7 +1521,7 @@
       <c r="C63" t="s">
         <v>6</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D63" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1345,7 +1535,7 @@
       <c r="C64" t="s">
         <v>6</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D64" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1359,7 +1549,7 @@
       <c r="C65" t="s">
         <v>6</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D65" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1373,7 +1563,7 @@
       <c r="C66" t="s">
         <v>6</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D66" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1387,7 +1577,7 @@
       <c r="C67" t="s">
         <v>6</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D67" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1401,7 +1591,7 @@
       <c r="C68" t="s">
         <v>6</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D68" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1415,7 +1605,7 @@
       <c r="C69" t="s">
         <v>6</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D69" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1429,7 +1619,7 @@
       <c r="C70" t="s">
         <v>6</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D70" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1443,7 +1633,7 @@
       <c r="C71" t="s">
         <v>6</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D71" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1457,7 +1647,7 @@
       <c r="C72" t="s">
         <v>6</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D72" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1471,7 +1661,7 @@
       <c r="C73" t="s">
         <v>6</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D73" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1485,7 +1675,7 @@
       <c r="C74" t="s">
         <v>6</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D74" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1499,7 +1689,7 @@
       <c r="C75" t="s">
         <v>6</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D75" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1513,7 +1703,7 @@
       <c r="C76" t="s">
         <v>6</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D76" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1527,7 +1717,7 @@
       <c r="C77" t="s">
         <v>6</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D77" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1541,7 +1731,7 @@
       <c r="C78" t="s">
         <v>6</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D78" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1555,7 +1745,7 @@
       <c r="C79" t="s">
         <v>6</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D79" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1569,7 +1759,7 @@
       <c r="C80" t="s">
         <v>6</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D80" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1583,7 +1773,7 @@
       <c r="C81" t="s">
         <v>6</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D81" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1597,7 +1787,7 @@
       <c r="C82" t="s">
         <v>6</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D82" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1611,7 +1801,7 @@
       <c r="C83" t="s">
         <v>6</v>
       </c>
-      <c r="D83" t="s">
+      <c r="D83" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1625,7 +1815,7 @@
       <c r="C84" t="s">
         <v>6</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D84" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1639,7 +1829,7 @@
       <c r="C85" t="s">
         <v>6</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D85" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1653,7 +1843,7 @@
       <c r="C86" t="s">
         <v>6</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D86" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1667,7 +1857,7 @@
       <c r="C87" t="s">
         <v>6</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D87" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1681,7 +1871,7 @@
       <c r="C88" t="s">
         <v>6</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D88" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1695,7 +1885,7 @@
       <c r="C89" t="s">
         <v>6</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D89" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1709,7 +1899,7 @@
       <c r="C90" t="s">
         <v>6</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D90" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1723,7 +1913,7 @@
       <c r="C91" t="s">
         <v>6</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D91" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1731,56 +1921,32 @@
       <c r="A92">
         <v>91</v>
       </c>
-      <c r="B92" t="s">
-        <v>6</v>
-      </c>
-      <c r="C92" t="s">
-        <v>6</v>
-      </c>
-      <c r="D92" t="s">
-        <v>6</v>
-      </c>
+      <c r="D92" s="2"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
-      <c r="B93" t="s">
-        <v>6</v>
-      </c>
-      <c r="C93" t="s">
-        <v>6</v>
-      </c>
-      <c r="D93" t="s">
-        <v>6</v>
-      </c>
+      <c r="D93" s="2"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
-      <c r="B94" t="s">
-        <v>6</v>
-      </c>
-      <c r="C94" t="s">
-        <v>6</v>
-      </c>
-      <c r="D94" t="s">
-        <v>6</v>
-      </c>
+      <c r="D94" s="2"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C95" t="s">
-        <v>6</v>
-      </c>
-      <c r="D95" t="s">
-        <v>6</v>
+        <v>22</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
@@ -1788,13 +1954,13 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C96" t="s">
-        <v>6</v>
-      </c>
-      <c r="D96" t="s">
-        <v>6</v>
+        <v>21</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
@@ -1802,13 +1968,13 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C97" t="s">
-        <v>6</v>
-      </c>
-      <c r="D97" t="s">
-        <v>6</v>
+        <v>23</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
@@ -1816,13 +1982,13 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C98" t="s">
-        <v>6</v>
-      </c>
-      <c r="D98" t="s">
-        <v>6</v>
+        <v>34</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
@@ -1830,13 +1996,13 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C99" t="s">
-        <v>6</v>
-      </c>
-      <c r="D99" t="s">
-        <v>6</v>
+        <v>35</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
@@ -1849,7 +2015,7 @@
       <c r="C100" t="s">
         <v>10</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D100" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1857,14 +2023,516 @@
       <c r="A101">
         <v>100</v>
       </c>
-      <c r="B101" t="s">
-        <v>7</v>
-      </c>
-      <c r="C101" t="s">
-        <v>8</v>
-      </c>
-      <c r="D101" s="1">
+      <c r="D101" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3F1A43D-A44F-F04B-8562-78C7F72CE509}">
+  <dimension ref="A1:A100"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>45455</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>45455</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>45455</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>45455</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>44930</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>45489</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>45455</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>45447</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>45455</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>45455</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>45138</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>45504</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>45504</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>45504</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>45504</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>45237</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>45237</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>45057</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>45411</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
         <v>45578</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>45578</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A92" s="2"/>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93" s="2"/>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94" s="2"/>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>